<commit_message>
added i2c pin-header, changed adc pinheader to 01x03 with vcc pin added
</commit_message>
<xml_diff>
--- a/datasheets/uc/pinout.xlsx
+++ b/datasheets/uc/pinout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzahedi\Documents\Git\RoboFriend\datasheets\uc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BDB691EC-4DA1-4889-BBBF-C92131C01452}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{08EEE680-5C1B-4A7D-9617-CD7FE221A485}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="110">
   <si>
     <t>Ports</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>GND</t>
-  </si>
-  <si>
-    <t>Vcc</t>
   </si>
   <si>
     <t>5V</t>
@@ -787,7 +784,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -833,14 +830,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
-      <i/>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -868,6 +857,40 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1028,108 +1051,129 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1520,832 +1564,832 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N10" sqref="N10"/>
+      <selection pane="bottomRight" sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="5.7109375" style="15"/>
-    <col min="3" max="9" width="8.5703125" style="15"/>
-    <col min="10" max="10" width="2.140625" style="15"/>
-    <col min="11" max="1001" width="8.5703125" style="15"/>
+    <col min="1" max="2" width="5.7109375" style="1"/>
+    <col min="3" max="9" width="8.5703125" style="1"/>
+    <col min="10" max="10" width="2.140625" style="1"/>
+    <col min="11" max="1001" width="8.5703125" style="1"/>
     <col min="1002" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="13" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
       <c r="I1"/>
       <c r="J1"/>
       <c r="K1"/>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="9" t="s">
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="26" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="16">
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="2">
         <v>1</v>
       </c>
-      <c r="G2" s="16">
+      <c r="G2" s="2">
         <v>2</v>
       </c>
-      <c r="H2" s="16">
+      <c r="H2" s="2">
         <v>3</v>
       </c>
       <c r="I2"/>
       <c r="J2"/>
       <c r="K2"/>
-      <c r="L2" s="16">
+      <c r="L2" s="2">
         <v>3</v>
       </c>
-      <c r="M2" s="16">
+      <c r="M2" s="2">
         <v>2</v>
       </c>
-      <c r="N2" s="16">
+      <c r="N2" s="2">
         <v>1</v>
       </c>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="8"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="26"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="17" t="s">
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="41" t="s">
         <v>7</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="17" t="s">
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="27"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="19" t="s">
+      <c r="D4" s="3">
+        <v>27</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="18">
+      <c r="F4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4"/>
+      <c r="K4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="P4" s="3">
+        <v>26</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5"/>
+      <c r="K5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="P5" s="3">
+        <v>25</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="20"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6"/>
+      <c r="K6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="18"/>
-      <c r="I4" s="19" t="s">
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J4"/>
-      <c r="K4" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="O4" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="P4" s="18">
-        <v>26</v>
-      </c>
-      <c r="Q4" s="19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="18">
-        <v>0</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5"/>
-      <c r="K5" s="19" t="s">
+      <c r="P6" s="3">
+        <v>24</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7"/>
+      <c r="K7" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="O7" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="P7" s="3">
+        <v>23</v>
+      </c>
+      <c r="Q7" s="39" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="22"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="3">
+        <v>3</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8"/>
+      <c r="K8" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O8" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="P8" s="3">
         <v>22</v>
       </c>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="O5" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="P5" s="18">
-        <v>25</v>
-      </c>
-      <c r="Q5" s="19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="18">
-        <v>1</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6"/>
-      <c r="K6" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="O6" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="P6" s="18">
-        <v>24</v>
-      </c>
-      <c r="Q6" s="19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="18">
-        <v>2</v>
-      </c>
-      <c r="E7" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" s="18"/>
-      <c r="I7" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="J7"/>
-      <c r="K7" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="O7" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="P7" s="18">
-        <v>23</v>
-      </c>
-      <c r="Q7" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="18">
-        <v>3</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="18" t="s">
+      <c r="Q8" s="39" t="s">
         <v>42</v>
-      </c>
-      <c r="H8" s="18"/>
-      <c r="I8" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="J8"/>
-      <c r="K8" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="O8" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="P8" s="18">
-        <v>22</v>
-      </c>
-      <c r="Q8" s="19" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9"/>
       <c r="B9"/>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="3">
+        <v>4</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="18">
-        <v>4</v>
-      </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18" t="s">
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9"/>
+      <c r="K9" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="J9"/>
-      <c r="K9" s="19" t="s">
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="O9" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="P9" s="18">
+      <c r="O9" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="P9" s="3">
         <v>21</v>
       </c>
-      <c r="Q9" s="19" t="s">
-        <v>47</v>
+      <c r="Q9" s="39" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10"/>
       <c r="B10"/>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="3">
+        <v>5</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="18">
-        <v>5</v>
-      </c>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18" t="s">
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J10"/>
+      <c r="K10" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="J10"/>
-      <c r="K10" s="19" t="s">
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="O10" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="P10" s="18">
+      <c r="O10" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="P10" s="3">
         <v>20</v>
       </c>
-      <c r="Q10" s="19" t="s">
-        <v>51</v>
+      <c r="Q10" s="39" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11"/>
       <c r="B11"/>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="3">
+        <v>6</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="18">
-        <v>6</v>
-      </c>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18" t="s">
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J11"/>
+      <c r="K11" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="J11"/>
-      <c r="K11" s="21" t="s">
+      <c r="L11" s="3"/>
+      <c r="M11" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18" t="s">
+      <c r="N11" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="N11" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18">
+      <c r="O11" s="3"/>
+      <c r="P11" s="3">
         <v>19</v>
       </c>
-      <c r="Q11" s="21" t="s">
-        <v>55</v>
+      <c r="Q11" s="6" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12"/>
       <c r="B12"/>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="3">
+        <v>7</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="18">
-        <v>7</v>
-      </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18" t="s">
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="J12"/>
+      <c r="K12" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="J12"/>
-      <c r="K12" s="21" t="s">
+      <c r="L12" s="3"/>
+      <c r="M12" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18" t="s">
+      <c r="N12" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="N12" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18">
+      <c r="O12" s="3"/>
+      <c r="P12" s="3">
         <v>18</v>
       </c>
-      <c r="Q12" s="21" t="s">
-        <v>60</v>
+      <c r="Q12" s="6" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13"/>
       <c r="B13"/>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="3">
+        <v>8</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="18">
-        <v>8</v>
-      </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="21" t="s">
-        <v>63</v>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="J13"/>
-      <c r="K13" s="17" t="s">
+      <c r="K13" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="17" t="s">
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17"/>
+      <c r="Q13" s="35" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14"/>
       <c r="B14"/>
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="3">
+        <v>9</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="J14"/>
+      <c r="K14" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="18">
-        <v>9</v>
-      </c>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="21" t="s">
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="36" t="s">
         <v>65</v>
-      </c>
-      <c r="J14"/>
-      <c r="K14" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="17" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15"/>
       <c r="B15"/>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="3">
+        <v>10</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="J15"/>
+      <c r="K15" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="18">
-        <v>10</v>
-      </c>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="22" t="s">
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O15" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="P15" s="3">
+        <v>38</v>
+      </c>
+      <c r="Q15" s="38" t="s">
         <v>67</v>
-      </c>
-      <c r="J15"/>
-      <c r="K15" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="O15" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="P15" s="18">
-        <v>38</v>
-      </c>
-      <c r="Q15" s="23" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16"/>
       <c r="B16"/>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="3">
+        <v>11</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="J16"/>
+      <c r="K16" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="18">
-        <v>11</v>
-      </c>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="22" t="s">
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="O16" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="P16" s="3">
+        <v>39</v>
+      </c>
+      <c r="Q16" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="J16"/>
-      <c r="K16" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18" t="s">
+    </row>
+    <row r="17" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C17" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="O16" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="P16" s="18">
-        <v>39</v>
-      </c>
-      <c r="Q16" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C17" s="34" t="s">
+      <c r="D17" s="3">
+        <v>12</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J17"/>
+      <c r="K17" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="18">
-        <v>12</v>
-      </c>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="22" t="s">
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="O17" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="P17" s="3">
+        <v>40</v>
+      </c>
+      <c r="Q17" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="J17"/>
-      <c r="K17" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="18" t="s">
+    </row>
+    <row r="18" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C18" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="O17" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="P17" s="18">
-        <v>40</v>
-      </c>
-      <c r="Q17" s="23" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C18" s="34" t="s">
+      <c r="D18" s="3">
+        <v>13</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D18" s="18">
-        <v>13</v>
-      </c>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18" t="s">
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="J18"/>
+      <c r="K18" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="J18"/>
-      <c r="K18" s="23" t="s">
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="18" t="s">
+      <c r="O18" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="P18" s="3">
+        <v>41</v>
+      </c>
+      <c r="Q18" s="38" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C19" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="O18" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="P18" s="18">
-        <v>41</v>
-      </c>
-      <c r="Q18" s="23" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C19" s="22" t="s">
+      <c r="D19" s="3">
+        <v>14</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="18">
-        <v>14</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="18" t="s">
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J19"/>
+      <c r="K19" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="J19"/>
-      <c r="K19" s="23" t="s">
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18" t="s">
+      <c r="O19" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P19" s="3">
+        <v>42</v>
+      </c>
+      <c r="Q19" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C20" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="O19" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="P19" s="18">
-        <v>42</v>
-      </c>
-      <c r="Q19" s="23" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C20" s="22" t="s">
+      <c r="D20" s="3">
+        <v>15</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D20" s="18">
-        <v>15</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="18" t="s">
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="J20"/>
+      <c r="K20" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="J20"/>
-      <c r="K20" s="23" t="s">
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18" t="s">
+      <c r="O20" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P20" s="3">
+        <v>43</v>
+      </c>
+      <c r="Q20" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C21" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="O20" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="P20" s="18">
-        <v>43</v>
-      </c>
-      <c r="Q20" s="23" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C21" s="22" t="s">
+      <c r="D21" s="3">
+        <v>16</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D21" s="18">
-        <v>16</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="18" t="s">
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J21"/>
+      <c r="K21" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="J21"/>
-      <c r="K21" s="23" t="s">
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18" t="s">
+      <c r="O21" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P21" s="3">
+        <v>44</v>
+      </c>
+      <c r="Q21" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C22" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="O21" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="P21" s="18">
-        <v>44</v>
-      </c>
-      <c r="Q21" s="23" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="22" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C22" s="22" t="s">
+      <c r="D22" s="3">
+        <v>17</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D22" s="18">
-        <v>17</v>
-      </c>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18" t="s">
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="J22"/>
+      <c r="K22" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="J22"/>
-      <c r="K22" s="23" t="s">
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="O22" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="P22" s="18">
+      <c r="O22" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P22" s="3">
         <v>45</v>
       </c>
-      <c r="Q22" s="23" t="s">
-        <v>95</v>
+      <c r="Q22" s="8" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="3:18" x14ac:dyDescent="0.25">
@@ -2355,7 +2399,7 @@
       <c r="F23"/>
       <c r="G23"/>
       <c r="H23"/>
-      <c r="J23" s="24"/>
+      <c r="J23" s="9"/>
       <c r="L23"/>
       <c r="M23"/>
       <c r="N23"/>
@@ -2364,218 +2408,198 @@
       <c r="Q23"/>
     </row>
     <row r="24" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C24" s="28" t="s">
+      <c r="C24" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+    </row>
+    <row r="25" spans="3:18" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28"/>
-      <c r="L24" s="25"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="26"/>
-      <c r="P24" s="26"/>
-      <c r="Q24" s="26"/>
-    </row>
-    <row r="25" spans="3:18" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="29" t="s">
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="L25" s="10"/>
+    </row>
+    <row r="26" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C26" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29"/>
-      <c r="L25" s="25"/>
-    </row>
-    <row r="26" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C26" s="28" t="s">
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="L26" s="12"/>
+    </row>
+    <row r="27" spans="3:18" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="10"/>
+    </row>
+    <row r="28" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C28" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28"/>
-      <c r="L26" s="27"/>
-    </row>
-    <row r="27" spans="3:18" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="30" t="s">
-        <v>110</v>
-      </c>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="30"/>
-      <c r="L27" s="25"/>
-      <c r="M27" s="26"/>
-      <c r="N27" s="26"/>
-      <c r="O27" s="26"/>
-      <c r="P27" s="26"/>
-      <c r="Q27" s="26"/>
-      <c r="R27" s="25"/>
-    </row>
-    <row r="28" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C28" s="28" t="s">
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
+    </row>
+    <row r="29" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C29" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="L28" s="25"/>
-      <c r="M28" s="25"/>
-      <c r="N28" s="25"/>
-      <c r="O28" s="25"/>
-      <c r="P28" s="25"/>
-      <c r="Q28" s="25"/>
-      <c r="R28" s="25"/>
-    </row>
-    <row r="29" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C29" s="28" t="s">
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="10"/>
+    </row>
+    <row r="30" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C30" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="28"/>
-      <c r="L29" s="25"/>
-      <c r="M29" s="25"/>
-      <c r="N29" s="25"/>
-      <c r="O29" s="25"/>
-      <c r="P29" s="25"/>
-      <c r="Q29" s="25"/>
-      <c r="R29" s="25"/>
-    </row>
-    <row r="30" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C30" s="28" t="s">
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="L30" s="10"/>
+    </row>
+    <row r="31" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C31" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
-      <c r="L30" s="25"/>
-    </row>
-    <row r="31" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C31" s="28" t="s">
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="L31" s="10"/>
+    </row>
+    <row r="32" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C32" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="D31" s="28"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="28"/>
-      <c r="L31" s="25"/>
-    </row>
-    <row r="32" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C32" s="28" t="s">
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="L32" s="10"/>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C33" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="D32" s="28"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="28"/>
-      <c r="L32" s="25"/>
-    </row>
-    <row r="33" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C33" s="28" t="s">
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="L33" s="10"/>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C34" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="D33" s="28"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
-      <c r="L33" s="25"/>
-    </row>
-    <row r="34" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C34" s="28" t="s">
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="L34" s="10"/>
+    </row>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C35" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="28"/>
-      <c r="G34" s="28"/>
-      <c r="H34" s="28"/>
-      <c r="I34" s="28"/>
-      <c r="L34" s="25"/>
-    </row>
-    <row r="35" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C35" s="28" t="s">
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="L35" s="10"/>
+    </row>
+    <row r="36" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C36" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="D35" s="28"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="28"/>
-      <c r="I35" s="28"/>
-      <c r="L35" s="25"/>
-    </row>
-    <row r="36" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C36" s="28" t="s">
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="L36" s="10"/>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C37" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="D36" s="28"/>
-      <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="28"/>
-      <c r="H36" s="28"/>
-      <c r="I36" s="28"/>
-      <c r="L36" s="25"/>
-    </row>
-    <row r="37" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C37" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="D37" s="28"/>
-      <c r="E37" s="28"/>
-      <c r="F37" s="28"/>
-      <c r="G37" s="28"/>
-      <c r="H37" s="28"/>
-      <c r="I37" s="28"/>
-      <c r="L37" s="25"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="16"/>
+      <c r="L37" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="C33:I33"/>
-    <mergeCell ref="C34:I34"/>
-    <mergeCell ref="C35:I35"/>
-    <mergeCell ref="C36:I36"/>
-    <mergeCell ref="C37:I37"/>
-    <mergeCell ref="C28:I28"/>
-    <mergeCell ref="C29:I29"/>
-    <mergeCell ref="C30:I30"/>
-    <mergeCell ref="C31:I31"/>
-    <mergeCell ref="C32:I32"/>
-    <mergeCell ref="L14:P14"/>
-    <mergeCell ref="C24:I24"/>
-    <mergeCell ref="C25:I25"/>
-    <mergeCell ref="C26:I26"/>
-    <mergeCell ref="C27:I27"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="L13:P13"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="P1:P2"/>
@@ -2589,6 +2613,26 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:H1"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="L13:P13"/>
+    <mergeCell ref="L14:P14"/>
+    <mergeCell ref="C24:I24"/>
+    <mergeCell ref="C25:I25"/>
+    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="C27:I27"/>
+    <mergeCell ref="C28:I28"/>
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="C30:I30"/>
+    <mergeCell ref="C31:I31"/>
+    <mergeCell ref="C32:I32"/>
+    <mergeCell ref="C33:I33"/>
+    <mergeCell ref="C34:I34"/>
+    <mergeCell ref="C35:I35"/>
+    <mergeCell ref="C36:I36"/>
+    <mergeCell ref="C37:I37"/>
   </mergeCells>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
adding simulations moduls for the paper and new pinout table
</commit_message>
<xml_diff>
--- a/datasheets/uc/pinout.xlsx
+++ b/datasheets/uc/pinout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzahedi\Documents\Git\RoboFriend\datasheets\uc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{08EEE680-5C1B-4A7D-9617-CD7FE221A485}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9F3A022D-673B-499A-8836-AC280E3AD9C4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -34,15 +34,9 @@
     <t>Ports</t>
   </si>
   <si>
-    <t>IO</t>
-  </si>
-  <si>
     <t>#</t>
   </si>
   <si>
-    <t>Pin</t>
-  </si>
-  <si>
     <t>Standard Function</t>
   </si>
   <si>
@@ -778,13 +772,19 @@
   </si>
   <si>
     <t>MISO: SPI Bus Master Input/Slave Output</t>
+  </si>
+  <si>
+    <t>Port Pin</t>
+  </si>
+  <si>
+    <t>Alternate Function</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -851,44 +851,14 @@
       <family val="2"/>
     </font>
     <font>
-      <strike/>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <i/>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <i/>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -943,7 +913,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1001,21 +971,6 @@
       <top style="thin">
         <color rgb="FFFFFFFF"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -1051,30 +1006,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1089,92 +1029,77 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1560,7 +1485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:ALM37"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -1577,47 +1502,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="30" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="E1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="F1" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
       <c r="I1"/>
       <c r="J1"/>
       <c r="K1"/>
-      <c r="L1" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="P1" s="25" t="s">
+      <c r="L1" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="26" t="s">
+      <c r="P1" s="13" t="s">
         <v>1</v>
       </c>
+      <c r="Q1" s="18" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="2" spans="1:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="19"/>
       <c r="E2" s="31"/>
       <c r="F2" s="2">
         <v>1</v>
@@ -1640,756 +1565,756 @@
       <c r="N2" s="2">
         <v>1</v>
       </c>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="26"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="18"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3"/>
+      <c r="K3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="28" t="s">
         <v>7</v>
-      </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3"/>
-      <c r="K3" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="35" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="4" t="s">
-        <v>9</v>
       </c>
       <c r="D4" s="3">
         <v>27</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="H4" s="3"/>
+      <c r="I4" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4"/>
+      <c r="K4" s="28" t="s">
         <v>11</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4"/>
-      <c r="K4" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="P4" s="3">
         <v>26</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="Q4" s="28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="B5" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>17</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="I5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5"/>
+      <c r="K5" s="28" t="s">
         <v>19</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5"/>
-      <c r="K5" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="P5" s="3">
         <v>25</v>
       </c>
-      <c r="Q5" s="4" t="s">
+      <c r="Q5" s="28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="21"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="9" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="40" t="s">
-        <v>23</v>
       </c>
       <c r="D6" s="3">
         <v>1</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="I6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6"/>
+      <c r="K6" s="28" t="s">
         <v>25</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6"/>
-      <c r="K6" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="P6" s="3">
         <v>24</v>
       </c>
-      <c r="Q6" s="4" t="s">
+      <c r="Q6" s="28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="B7" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>29</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="D7" s="3">
         <v>2</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="H7" s="3"/>
+      <c r="I7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7"/>
+      <c r="K7" s="28" t="s">
         <v>33</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="J7"/>
-      <c r="K7" s="39" t="s">
-        <v>35</v>
       </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="O7" s="37" t="s">
-        <v>37</v>
+        <v>34</v>
+      </c>
+      <c r="O7" s="12" t="s">
+        <v>35</v>
       </c>
       <c r="P7" s="3">
         <v>23</v>
       </c>
-      <c r="Q7" s="39" t="s">
-        <v>35</v>
+      <c r="Q7" s="28" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="5" t="s">
-        <v>38</v>
+      <c r="A8" s="23"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="D8" s="3">
         <v>3</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="H8" s="3"/>
+      <c r="I8" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8"/>
+      <c r="K8" s="28" t="s">
         <v>40</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J8"/>
-      <c r="K8" s="39" t="s">
-        <v>42</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="O8" s="37" t="s">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c r="O8" s="12" t="s">
+        <v>35</v>
       </c>
       <c r="P8" s="3">
         <v>22</v>
       </c>
-      <c r="Q8" s="39" t="s">
-        <v>42</v>
+      <c r="Q8" s="28" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9"/>
       <c r="B9"/>
-      <c r="C9" s="33" t="s">
-        <v>44</v>
+      <c r="C9" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="D9" s="3">
         <v>4</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9"/>
+      <c r="K9" s="28" t="s">
         <v>44</v>
-      </c>
-      <c r="J9"/>
-      <c r="K9" s="39" t="s">
-        <v>46</v>
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="O9" s="37" t="s">
-        <v>37</v>
+        <v>45</v>
+      </c>
+      <c r="O9" s="12" t="s">
+        <v>35</v>
       </c>
       <c r="P9" s="3">
         <v>21</v>
       </c>
-      <c r="Q9" s="39" t="s">
-        <v>46</v>
+      <c r="Q9" s="28" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10"/>
       <c r="B10"/>
-      <c r="C10" s="5" t="s">
-        <v>48</v>
+      <c r="C10" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="D10" s="3">
         <v>5</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10"/>
+      <c r="K10" s="28" t="s">
         <v>48</v>
-      </c>
-      <c r="J10"/>
-      <c r="K10" s="39" t="s">
-        <v>50</v>
       </c>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="O10" s="37" t="s">
-        <v>37</v>
+        <v>49</v>
+      </c>
+      <c r="O10" s="12" t="s">
+        <v>35</v>
       </c>
       <c r="P10" s="3">
         <v>20</v>
       </c>
-      <c r="Q10" s="39" t="s">
-        <v>50</v>
+      <c r="Q10" s="28" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11"/>
       <c r="B11"/>
-      <c r="C11" s="5" t="s">
-        <v>52</v>
+      <c r="C11" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="D11" s="3">
         <v>6</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="J11"/>
+      <c r="K11" s="29" t="s">
         <v>52</v>
-      </c>
-      <c r="J11"/>
-      <c r="K11" s="6" t="s">
-        <v>54</v>
       </c>
       <c r="L11" s="3"/>
       <c r="M11" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O11" s="3"/>
       <c r="P11" s="3">
         <v>19</v>
       </c>
-      <c r="Q11" s="6" t="s">
-        <v>54</v>
+      <c r="Q11" s="29" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12"/>
       <c r="B12"/>
-      <c r="C12" s="5" t="s">
-        <v>57</v>
+      <c r="C12" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="D12" s="3">
         <v>7</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="J12"/>
+      <c r="K12" s="29" t="s">
         <v>57</v>
-      </c>
-      <c r="J12"/>
-      <c r="K12" s="6" t="s">
-        <v>59</v>
       </c>
       <c r="L12" s="3"/>
       <c r="M12" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="O12" s="3"/>
       <c r="P12" s="3">
         <v>18</v>
       </c>
-      <c r="Q12" s="6" t="s">
-        <v>59</v>
+      <c r="Q12" s="29" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13"/>
       <c r="B13"/>
-      <c r="C13" s="14" t="s">
-        <v>62</v>
+      <c r="C13" s="29" t="s">
+        <v>60</v>
       </c>
       <c r="D13" s="3">
         <v>8</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="6" t="s">
-        <v>62</v>
+      <c r="I13" s="29" t="s">
+        <v>60</v>
       </c>
       <c r="J13"/>
-      <c r="K13" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="17"/>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="35" t="s">
-        <v>7</v>
+      <c r="K13" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="11" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14"/>
       <c r="B14"/>
-      <c r="C14" s="14" t="s">
-        <v>64</v>
+      <c r="C14" s="29" t="s">
+        <v>62</v>
       </c>
       <c r="D14" s="3">
         <v>9</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
-      <c r="I14" s="6" t="s">
-        <v>64</v>
+      <c r="I14" s="29" t="s">
+        <v>62</v>
       </c>
       <c r="J14"/>
-      <c r="K14" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="36" t="s">
-        <v>65</v>
+      <c r="K14" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="11" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15"/>
       <c r="B15"/>
-      <c r="C15" s="15" t="s">
-        <v>66</v>
+      <c r="C15" s="10" t="s">
+        <v>64</v>
       </c>
       <c r="D15" s="3">
         <v>10</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
-      <c r="I15" s="7" t="s">
-        <v>66</v>
+      <c r="I15" s="10" t="s">
+        <v>64</v>
       </c>
       <c r="J15"/>
-      <c r="K15" s="38" t="s">
-        <v>67</v>
+      <c r="K15" s="30" t="s">
+        <v>65</v>
       </c>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="O15" s="37" t="s">
-        <v>69</v>
+        <v>66</v>
+      </c>
+      <c r="O15" s="12" t="s">
+        <v>67</v>
       </c>
       <c r="P15" s="3">
         <v>38</v>
       </c>
-      <c r="Q15" s="38" t="s">
-        <v>67</v>
+      <c r="Q15" s="30" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16"/>
       <c r="B16"/>
-      <c r="C16" s="15" t="s">
-        <v>70</v>
+      <c r="C16" s="10" t="s">
+        <v>68</v>
       </c>
       <c r="D16" s="3">
         <v>11</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
-      <c r="I16" s="7" t="s">
-        <v>70</v>
+      <c r="I16" s="10" t="s">
+        <v>68</v>
       </c>
       <c r="J16"/>
-      <c r="K16" s="38" t="s">
-        <v>71</v>
+      <c r="K16" s="30" t="s">
+        <v>69</v>
       </c>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="O16" s="37" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="O16" s="12" t="s">
+        <v>67</v>
       </c>
       <c r="P16" s="3">
         <v>39</v>
       </c>
-      <c r="Q16" s="38" t="s">
+      <c r="Q16" s="30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C17" s="10" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C17" s="15" t="s">
-        <v>73</v>
       </c>
       <c r="D17" s="3">
         <v>12</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="7" t="s">
-        <v>73</v>
+      <c r="I17" s="10" t="s">
+        <v>71</v>
       </c>
       <c r="J17"/>
-      <c r="K17" s="38" t="s">
-        <v>74</v>
+      <c r="K17" s="30" t="s">
+        <v>72</v>
       </c>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
       <c r="N17" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="O17" s="37" t="s">
-        <v>69</v>
+        <v>73</v>
+      </c>
+      <c r="O17" s="12" t="s">
+        <v>67</v>
       </c>
       <c r="P17" s="3">
         <v>40</v>
       </c>
-      <c r="Q17" s="38" t="s">
+      <c r="Q17" s="30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C18" s="10" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C18" s="7" t="s">
-        <v>76</v>
       </c>
       <c r="D18" s="3">
         <v>13</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="7" t="s">
+      <c r="I18" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="J18"/>
+      <c r="K18" s="30" t="s">
         <v>76</v>
-      </c>
-      <c r="J18"/>
-      <c r="K18" s="38" t="s">
-        <v>78</v>
       </c>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="O18" s="37" t="s">
-        <v>69</v>
+        <v>77</v>
+      </c>
+      <c r="O18" s="12" t="s">
+        <v>67</v>
       </c>
       <c r="P18" s="3">
         <v>41</v>
       </c>
-      <c r="Q18" s="38" t="s">
+      <c r="Q18" s="30" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C19" s="10" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C19" s="7" t="s">
-        <v>80</v>
       </c>
       <c r="D19" s="3">
         <v>14</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="7" t="s">
+      <c r="I19" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="J19"/>
+      <c r="K19" s="30" t="s">
         <v>80</v>
-      </c>
-      <c r="J19"/>
-      <c r="K19" s="8" t="s">
-        <v>82</v>
       </c>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
       <c r="N19" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P19" s="3">
         <v>42</v>
       </c>
-      <c r="Q19" s="8" t="s">
+      <c r="Q19" s="30" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C20" s="10" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C20" s="7" t="s">
-        <v>84</v>
       </c>
       <c r="D20" s="3">
         <v>15</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
-      <c r="I20" s="7" t="s">
+      <c r="I20" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="J20"/>
+      <c r="K20" s="30" t="s">
         <v>84</v>
-      </c>
-      <c r="J20"/>
-      <c r="K20" s="8" t="s">
-        <v>86</v>
       </c>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P20" s="3">
         <v>43</v>
       </c>
-      <c r="Q20" s="8" t="s">
+      <c r="Q20" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C21" s="10" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="21" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C21" s="7" t="s">
-        <v>88</v>
       </c>
       <c r="D21" s="3">
         <v>16</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
-      <c r="I21" s="7" t="s">
+      <c r="I21" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="J21"/>
+      <c r="K21" s="30" t="s">
         <v>88</v>
-      </c>
-      <c r="J21"/>
-      <c r="K21" s="8" t="s">
-        <v>90</v>
       </c>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P21" s="3">
         <v>44</v>
       </c>
-      <c r="Q21" s="8" t="s">
+      <c r="Q21" s="30" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C22" s="10" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="22" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C22" s="34" t="s">
-        <v>92</v>
       </c>
       <c r="D22" s="3">
         <v>17</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="7" t="s">
+      <c r="I22" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="J22"/>
+      <c r="K22" s="30" t="s">
         <v>92</v>
-      </c>
-      <c r="J22"/>
-      <c r="K22" s="8" t="s">
-        <v>94</v>
       </c>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
       <c r="N22" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P22" s="3">
         <v>45</v>
       </c>
-      <c r="Q22" s="8" t="s">
-        <v>94</v>
+      <c r="Q22" s="30" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="3:18" x14ac:dyDescent="0.25">
@@ -2399,7 +2324,7 @@
       <c r="F23"/>
       <c r="G23"/>
       <c r="H23"/>
-      <c r="J23" s="9"/>
+      <c r="J23" s="4"/>
       <c r="L23"/>
       <c r="M23"/>
       <c r="N23"/>
@@ -2408,198 +2333,218 @@
       <c r="Q23"/>
     </row>
     <row r="24" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+    </row>
+    <row r="25" spans="3:18" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="L25" s="5"/>
+    </row>
+    <row r="26" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C26" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="11"/>
-      <c r="N24" s="11"/>
-      <c r="O24" s="11"/>
-      <c r="P24" s="11"/>
-      <c r="Q24" s="11"/>
-    </row>
-    <row r="25" spans="3:18" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="18" t="s">
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+      <c r="L26" s="7"/>
+    </row>
+    <row r="27" spans="3:18" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="5"/>
+    </row>
+    <row r="28" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C28" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
-      <c r="L25" s="10"/>
-    </row>
-    <row r="26" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C26" s="16" t="s">
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+    </row>
+    <row r="29" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C29" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="L26" s="12"/>
-    </row>
-    <row r="27" spans="3:18" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="19"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="11"/>
-      <c r="N27" s="11"/>
-      <c r="O27" s="11"/>
-      <c r="P27" s="11"/>
-      <c r="Q27" s="11"/>
-      <c r="R27" s="10"/>
-    </row>
-    <row r="28" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C28" s="16" t="s">
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+    </row>
+    <row r="30" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C30" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
-      <c r="N28" s="10"/>
-      <c r="O28" s="10"/>
-      <c r="P28" s="10"/>
-      <c r="Q28" s="10"/>
-      <c r="R28" s="10"/>
-    </row>
-    <row r="29" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C29" s="16" t="s">
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="25"/>
+      <c r="I30" s="25"/>
+      <c r="L30" s="5"/>
+    </row>
+    <row r="31" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C31" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
-      <c r="N29" s="10"/>
-      <c r="O29" s="10"/>
-      <c r="P29" s="10"/>
-      <c r="Q29" s="10"/>
-      <c r="R29" s="10"/>
-    </row>
-    <row r="30" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C30" s="16" t="s">
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="25"/>
+      <c r="L31" s="5"/>
+    </row>
+    <row r="32" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C32" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="L30" s="10"/>
-    </row>
-    <row r="31" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C31" s="16" t="s">
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="25"/>
+      <c r="L32" s="5"/>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C33" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="16"/>
-      <c r="L31" s="10"/>
-    </row>
-    <row r="32" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C32" s="16" t="s">
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="25"/>
+      <c r="L33" s="5"/>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C34" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
-      <c r="H32" s="16"/>
-      <c r="I32" s="16"/>
-      <c r="L32" s="10"/>
-    </row>
-    <row r="33" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C33" s="16" t="s">
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="25"/>
+      <c r="L34" s="5"/>
+    </row>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C35" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
-      <c r="I33" s="16"/>
-      <c r="L33" s="10"/>
-    </row>
-    <row r="34" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C34" s="16" t="s">
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="25"/>
+      <c r="I35" s="25"/>
+      <c r="L35" s="5"/>
+    </row>
+    <row r="36" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C36" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16"/>
-      <c r="L34" s="10"/>
-    </row>
-    <row r="35" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C35" s="16" t="s">
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="25"/>
+      <c r="I36" s="25"/>
+      <c r="L36" s="5"/>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C37" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="L35" s="10"/>
-    </row>
-    <row r="36" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C36" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="16"/>
-      <c r="I36" s="16"/>
-      <c r="L36" s="10"/>
-    </row>
-    <row r="37" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C37" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="16"/>
-      <c r="I37" s="16"/>
-      <c r="L37" s="10"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="25"/>
+      <c r="I37" s="25"/>
+      <c r="L37" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="C33:I33"/>
+    <mergeCell ref="C34:I34"/>
+    <mergeCell ref="C35:I35"/>
+    <mergeCell ref="C36:I36"/>
+    <mergeCell ref="C37:I37"/>
+    <mergeCell ref="C28:I28"/>
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="C30:I30"/>
+    <mergeCell ref="C31:I31"/>
+    <mergeCell ref="C32:I32"/>
+    <mergeCell ref="L14:P14"/>
+    <mergeCell ref="C24:I24"/>
+    <mergeCell ref="C25:I25"/>
+    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="C27:I27"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="L13:P13"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="P1:P2"/>
@@ -2613,26 +2558,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:H1"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="L13:P13"/>
-    <mergeCell ref="L14:P14"/>
-    <mergeCell ref="C24:I24"/>
-    <mergeCell ref="C25:I25"/>
-    <mergeCell ref="C26:I26"/>
-    <mergeCell ref="C27:I27"/>
-    <mergeCell ref="C28:I28"/>
-    <mergeCell ref="C29:I29"/>
-    <mergeCell ref="C30:I30"/>
-    <mergeCell ref="C31:I31"/>
-    <mergeCell ref="C32:I32"/>
-    <mergeCell ref="C33:I33"/>
-    <mergeCell ref="C34:I34"/>
-    <mergeCell ref="C35:I35"/>
-    <mergeCell ref="C36:I36"/>
-    <mergeCell ref="C37:I37"/>
   </mergeCells>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
added pegel shifter for uart and i2c, added pegel shifter simuluation file
</commit_message>
<xml_diff>
--- a/datasheets/uc/pinout.xlsx
+++ b/datasheets/uc/pinout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzahedi\Documents\Git\RoboFriend\datasheets\uc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6B452EAB-FFFA-47F6-B742-9EE27279380A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8029D9ED-E9B8-4789-AB59-BE3F1940DE19}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -1180,65 +1180,65 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1645,56 +1645,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="38" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
       <c r="J1"/>
       <c r="K1"/>
       <c r="L1"/>
-      <c r="M1" s="40" t="s">
+      <c r="M1" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="41" t="s">
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="33" t="s">
+      <c r="Q1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="33" t="s">
+      <c r="R1" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="S1" s="38" t="s">
+      <c r="S1" s="32" t="s">
         <v>108</v>
       </c>
       <c r="T1"/>
     </row>
     <row r="2" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="37"/>
-      <c r="B2" s="37"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
       <c r="G2" s="2">
         <v>1</v>
       </c>
@@ -1716,17 +1716,17 @@
       <c r="O2" s="2">
         <v>1</v>
       </c>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="38"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="32"/>
       <c r="T2"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="34" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -1735,11 +1735,11 @@
       <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
       <c r="J3" s="3" t="s">
         <v>5</v>
       </c>
@@ -1747,11 +1747,11 @@
       <c r="L3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="35"/>
       <c r="R3" s="18" t="s">
         <v>6</v>
       </c>
@@ -1761,12 +1761,12 @@
       <c r="T3"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="36"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="25" t="s">
         <v>111</v>
       </c>
       <c r="E4" s="4">
@@ -1809,16 +1809,16 @@
       <c r="T4"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="38" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="43" t="s">
+      <c r="D5" s="26" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="4">
@@ -1863,12 +1863,12 @@
       <c r="T5"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="29"/>
+      <c r="A6" s="37"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="43" t="s">
+      <c r="D6" s="26" t="s">
         <v>23</v>
       </c>
       <c r="E6" s="4">
@@ -1913,16 +1913,16 @@
       <c r="T6"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="40" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="42" t="s">
+      <c r="D7" s="25" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="4">
@@ -1947,7 +1947,7 @@
       </c>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
-      <c r="O7" s="18" t="s">
+      <c r="O7" s="21" t="s">
         <v>34</v>
       </c>
       <c r="P7" s="4" t="s">
@@ -1965,12 +1965,12 @@
       <c r="T7"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="31"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="40"/>
       <c r="C8" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="25" t="s">
         <v>37</v>
       </c>
       <c r="E8" s="4">
@@ -1995,7 +1995,7 @@
       </c>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
-      <c r="O8" s="18" t="s">
+      <c r="O8" s="21" t="s">
         <v>41</v>
       </c>
       <c r="P8" s="4" t="s">
@@ -2016,7 +2016,7 @@
       <c r="C9" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="25" t="s">
         <v>112</v>
       </c>
       <c r="E9" s="4">
@@ -2037,7 +2037,7 @@
       </c>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
-      <c r="O9" s="18" t="s">
+      <c r="O9" s="21" t="s">
         <v>45</v>
       </c>
       <c r="P9" s="4" t="s">
@@ -2058,7 +2058,7 @@
       <c r="C10" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="25" t="s">
         <v>113</v>
       </c>
       <c r="E10" s="4">
@@ -2079,7 +2079,7 @@
       </c>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
-      <c r="O10" s="18" t="s">
+      <c r="O10" s="21" t="s">
         <v>49</v>
       </c>
       <c r="P10" s="4" t="s">
@@ -2100,7 +2100,7 @@
       <c r="C11" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="25" t="s">
         <v>115</v>
       </c>
       <c r="E11" s="4">
@@ -2142,7 +2142,7 @@
       <c r="C12" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="25" t="s">
         <v>114</v>
       </c>
       <c r="E12" s="4">
@@ -2165,7 +2165,7 @@
       <c r="N12" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="O12" s="18" t="s">
+      <c r="O12" s="21" t="s">
         <v>59</v>
       </c>
       <c r="P12" s="4"/>
@@ -2184,7 +2184,7 @@
       <c r="C13" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="42" t="s">
+      <c r="D13" s="25" t="s">
         <v>128</v>
       </c>
       <c r="E13" s="4">
@@ -2203,11 +2203,11 @@
       <c r="L13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="M13" s="26"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="26"/>
-      <c r="P13" s="26"/>
-      <c r="Q13" s="26"/>
+      <c r="M13" s="35"/>
+      <c r="N13" s="35"/>
+      <c r="O13" s="35"/>
+      <c r="P13" s="35"/>
+      <c r="Q13" s="35"/>
       <c r="R13" s="18" t="s">
         <v>5</v>
       </c>
@@ -2220,7 +2220,7 @@
       <c r="C14" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="25" t="s">
         <v>131</v>
       </c>
       <c r="E14" s="4">
@@ -2236,18 +2236,18 @@
         <v>62</v>
       </c>
       <c r="K14"/>
-      <c r="L14" s="44" t="s">
+      <c r="L14" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
-      <c r="O14" s="26"/>
-      <c r="P14" s="26"/>
-      <c r="Q14" s="26"/>
+      <c r="M14" s="35"/>
+      <c r="N14" s="35"/>
+      <c r="O14" s="35"/>
+      <c r="P14" s="35"/>
+      <c r="Q14" s="35"/>
       <c r="R14" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="S14" s="44" t="s">
+      <c r="S14" s="27" t="s">
         <v>63</v>
       </c>
       <c r="T14"/>
@@ -2256,7 +2256,7 @@
       <c r="C15" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="25" t="s">
         <v>116</v>
       </c>
       <c r="E15" s="4">
@@ -2277,7 +2277,7 @@
       </c>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
-      <c r="O15" s="18" t="s">
+      <c r="O15" s="21" t="s">
         <v>66</v>
       </c>
       <c r="P15" s="21" t="s">
@@ -2298,7 +2298,7 @@
       <c r="C16" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="D16" s="42" t="s">
+      <c r="D16" s="25" t="s">
         <v>117</v>
       </c>
       <c r="E16" s="4">
@@ -2319,7 +2319,7 @@
       </c>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
-      <c r="O16" s="18" t="s">
+      <c r="O16" s="21" t="s">
         <v>70</v>
       </c>
       <c r="P16" s="21" t="s">
@@ -2340,7 +2340,7 @@
       <c r="C17" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="42" t="s">
+      <c r="D17" s="25" t="s">
         <v>118</v>
       </c>
       <c r="E17" s="4">
@@ -2361,7 +2361,7 @@
       </c>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
-      <c r="O17" s="18" t="s">
+      <c r="O17" s="21" t="s">
         <v>73</v>
       </c>
       <c r="P17" s="21" t="s">
@@ -2382,7 +2382,7 @@
       <c r="C18" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="42" t="s">
+      <c r="D18" s="25" t="s">
         <v>119</v>
       </c>
       <c r="E18" s="4">
@@ -2403,7 +2403,7 @@
       </c>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
-      <c r="O18" s="18" t="s">
+      <c r="O18" s="21" t="s">
         <v>77</v>
       </c>
       <c r="P18" s="21" t="s">
@@ -2424,7 +2424,7 @@
       <c r="C19" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="D19" s="42" t="s">
+      <c r="D19" s="25" t="s">
         <v>120</v>
       </c>
       <c r="E19" s="4">
@@ -2447,7 +2447,7 @@
       </c>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
-      <c r="O19" s="18" t="s">
+      <c r="O19" s="21" t="s">
         <v>81</v>
       </c>
       <c r="P19" s="21" t="s">
@@ -2468,7 +2468,7 @@
       <c r="C20" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="D20" s="42" t="s">
+      <c r="D20" s="25" t="s">
         <v>121</v>
       </c>
       <c r="E20" s="4">
@@ -2491,7 +2491,7 @@
       </c>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
-      <c r="O20" s="18" t="s">
+      <c r="O20" s="21" t="s">
         <v>85</v>
       </c>
       <c r="P20" s="21" t="s">
@@ -2512,7 +2512,7 @@
       <c r="C21" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="D21" s="42" t="s">
+      <c r="D21" s="25" t="s">
         <v>130</v>
       </c>
       <c r="E21" s="4">
@@ -2554,7 +2554,7 @@
       <c r="C22" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="D22" s="42" t="s">
+      <c r="D22" s="25" t="s">
         <v>129</v>
       </c>
       <c r="E22" s="4">
@@ -2610,16 +2610,16 @@
       <c r="T23"/>
     </row>
     <row r="24" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="25"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="41"/>
+      <c r="J24" s="41"/>
       <c r="M24" s="15"/>
       <c r="N24" s="16"/>
       <c r="O24" s="16"/>
@@ -2630,16 +2630,16 @@
       <c r="T24"/>
     </row>
     <row r="25" spans="3:20" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="27" t="s">
+      <c r="C25" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="27"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="42"/>
       <c r="M25" s="15"/>
       <c r="N25"/>
       <c r="O25"/>
@@ -2650,16 +2650,16 @@
       <c r="T25"/>
     </row>
     <row r="26" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C26" s="25" t="s">
+      <c r="C26" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="25"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="41"/>
+      <c r="J26" s="41"/>
       <c r="M26" s="17"/>
       <c r="N26"/>
       <c r="O26"/>
@@ -2670,16 +2670,16 @@
       <c r="T26"/>
     </row>
     <row r="27" spans="3:20" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="27" t="s">
+      <c r="C27" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="27"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
       <c r="M27" s="15"/>
       <c r="N27" s="16"/>
       <c r="O27" s="16"/>
@@ -2690,16 +2690,16 @@
       <c r="T27" s="15"/>
     </row>
     <row r="28" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C28" s="25" t="s">
+      <c r="C28" s="41" t="s">
         <v>98</v>
       </c>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
+      <c r="G28" s="41"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="41"/>
+      <c r="J28" s="41"/>
       <c r="M28" s="15"/>
       <c r="N28" s="15"/>
       <c r="O28" s="15"/>
@@ -2710,16 +2710,16 @@
       <c r="T28" s="15"/>
     </row>
     <row r="29" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C29" s="25" t="s">
+      <c r="C29" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="41"/>
+      <c r="J29" s="41"/>
       <c r="M29" s="15"/>
       <c r="N29" s="15"/>
       <c r="O29" s="15"/>
@@ -2730,111 +2730,131 @@
       <c r="T29" s="15"/>
     </row>
     <row r="30" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C30" s="25" t="s">
+      <c r="C30" s="41" t="s">
         <v>100</v>
       </c>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="25"/>
-      <c r="I30" s="25"/>
-      <c r="J30" s="25"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="41"/>
+      <c r="J30" s="41"/>
       <c r="M30" s="15"/>
     </row>
     <row r="31" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C31" s="25" t="s">
+      <c r="C31" s="41" t="s">
         <v>101</v>
       </c>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="25"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="41"/>
+      <c r="J31" s="41"/>
       <c r="M31" s="15"/>
     </row>
     <row r="32" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C32" s="25" t="s">
+      <c r="C32" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="25"/>
-      <c r="J32" s="25"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="41"/>
+      <c r="J32" s="41"/>
       <c r="M32" s="15"/>
     </row>
     <row r="33" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C33" s="25" t="s">
+      <c r="C33" s="41" t="s">
         <v>103</v>
       </c>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="25"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="41"/>
+      <c r="H33" s="41"/>
+      <c r="I33" s="41"/>
+      <c r="J33" s="41"/>
       <c r="M33" s="15"/>
     </row>
     <row r="34" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C34" s="25" t="s">
+      <c r="C34" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="41"/>
+      <c r="F34" s="41"/>
+      <c r="G34" s="41"/>
+      <c r="H34" s="41"/>
+      <c r="I34" s="41"/>
+      <c r="J34" s="41"/>
       <c r="M34" s="15"/>
     </row>
     <row r="35" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C35" s="25" t="s">
+      <c r="C35" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="25"/>
+      <c r="D35" s="41"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="41"/>
+      <c r="G35" s="41"/>
+      <c r="H35" s="41"/>
+      <c r="I35" s="41"/>
+      <c r="J35" s="41"/>
       <c r="M35" s="15"/>
     </row>
     <row r="36" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C36" s="25" t="s">
+      <c r="C36" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25"/>
-      <c r="H36" s="25"/>
-      <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
+      <c r="D36" s="41"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
+      <c r="G36" s="41"/>
+      <c r="H36" s="41"/>
+      <c r="I36" s="41"/>
+      <c r="J36" s="41"/>
       <c r="M36" s="15"/>
     </row>
     <row r="37" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C37" s="25" t="s">
+      <c r="C37" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="25"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
+      <c r="G37" s="41"/>
+      <c r="H37" s="41"/>
+      <c r="I37" s="41"/>
+      <c r="J37" s="41"/>
       <c r="M37" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="C33:J33"/>
+    <mergeCell ref="C34:J34"/>
+    <mergeCell ref="C35:J35"/>
+    <mergeCell ref="C36:J36"/>
+    <mergeCell ref="C37:J37"/>
+    <mergeCell ref="C28:J28"/>
+    <mergeCell ref="C29:J29"/>
+    <mergeCell ref="C30:J30"/>
+    <mergeCell ref="C31:J31"/>
+    <mergeCell ref="C32:J32"/>
+    <mergeCell ref="M14:Q14"/>
+    <mergeCell ref="C24:J24"/>
+    <mergeCell ref="C25:J25"/>
+    <mergeCell ref="C26:J26"/>
+    <mergeCell ref="C27:J27"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="M13:Q13"/>
     <mergeCell ref="M1:O1"/>
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="Q1:Q2"/>
@@ -2850,26 +2870,6 @@
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="R1:R2"/>
     <mergeCell ref="D1:D2"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="M13:Q13"/>
-    <mergeCell ref="M14:Q14"/>
-    <mergeCell ref="C24:J24"/>
-    <mergeCell ref="C25:J25"/>
-    <mergeCell ref="C26:J26"/>
-    <mergeCell ref="C27:J27"/>
-    <mergeCell ref="C28:J28"/>
-    <mergeCell ref="C29:J29"/>
-    <mergeCell ref="C30:J30"/>
-    <mergeCell ref="C31:J31"/>
-    <mergeCell ref="C32:J32"/>
-    <mergeCell ref="C33:J33"/>
-    <mergeCell ref="C34:J34"/>
-    <mergeCell ref="C35:J35"/>
-    <mergeCell ref="C36:J36"/>
-    <mergeCell ref="C37:J37"/>
   </mergeCells>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2897,49 +2897,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="38" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
       <c r="I1"/>
       <c r="J1"/>
       <c r="K1"/>
-      <c r="L1" s="32" t="s">
+      <c r="L1" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="34" t="s">
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="33" t="s">
+      <c r="P1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" s="34" t="s">
+      <c r="Q1" s="44" t="s">
         <v>108</v>
       </c>
       <c r="R1"/>
     </row>
     <row r="2" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="37"/>
-      <c r="B2" s="37"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
       <c r="F2" s="2">
         <v>1</v>
       </c>
@@ -2961,26 +2961,26 @@
       <c r="N2" s="2">
         <v>1</v>
       </c>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
       <c r="R2"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="34" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
       <c r="I3" s="10" t="s">
         <v>5</v>
       </c>
@@ -2988,19 +2988,19 @@
       <c r="K3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
       <c r="Q3" s="10" t="s">
         <v>6</v>
       </c>
       <c r="R3"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="36"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
@@ -3041,10 +3041,10 @@
       <c r="R4"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="38" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -3089,8 +3089,8 @@
       <c r="R5"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="29"/>
+      <c r="A6" s="37"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="7" t="s">
         <v>21</v>
       </c>
@@ -3133,10 +3133,10 @@
       <c r="R6"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="40" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -3179,8 +3179,8 @@
       <c r="R7"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="31"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="40"/>
       <c r="C8" s="7" t="s">
         <v>36</v>
       </c>
@@ -3384,11 +3384,11 @@
       <c r="K13" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="L13" s="26"/>
-      <c r="M13" s="26"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="26"/>
-      <c r="P13" s="26"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="35"/>
+      <c r="N13" s="35"/>
+      <c r="O13" s="35"/>
+      <c r="P13" s="35"/>
       <c r="Q13" s="10" t="s">
         <v>5</v>
       </c>
@@ -3414,11 +3414,11 @@
       <c r="K14" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
-      <c r="O14" s="26"/>
-      <c r="P14" s="26"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="35"/>
+      <c r="N14" s="35"/>
+      <c r="O14" s="35"/>
+      <c r="P14" s="35"/>
       <c r="Q14" s="10" t="s">
         <v>63</v>
       </c>
@@ -3736,15 +3736,15 @@
       <c r="R23"/>
     </row>
     <row r="24" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="25"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="41"/>
       <c r="L24" s="15"/>
       <c r="M24" s="16"/>
       <c r="N24" s="16"/>
@@ -3754,15 +3754,15 @@
       <c r="R24"/>
     </row>
     <row r="25" spans="3:18" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="27" t="s">
+      <c r="C25" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="42"/>
       <c r="L25" s="15"/>
       <c r="M25"/>
       <c r="N25"/>
@@ -3772,15 +3772,15 @@
       <c r="R25"/>
     </row>
     <row r="26" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C26" s="25" t="s">
+      <c r="C26" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="41"/>
       <c r="L26" s="17"/>
       <c r="M26"/>
       <c r="N26"/>
@@ -3790,15 +3790,15 @@
       <c r="R26"/>
     </row>
     <row r="27" spans="3:18" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="27" t="s">
+      <c r="C27" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="27"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
       <c r="L27" s="15"/>
       <c r="M27" s="16"/>
       <c r="N27" s="16"/>
@@ -3808,15 +3808,15 @@
       <c r="R27" s="15"/>
     </row>
     <row r="28" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C28" s="25" t="s">
+      <c r="C28" s="41" t="s">
         <v>98</v>
       </c>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
+      <c r="G28" s="41"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="41"/>
       <c r="L28" s="15"/>
       <c r="M28" s="15"/>
       <c r="N28" s="15"/>
@@ -3826,15 +3826,15 @@
       <c r="R28" s="15"/>
     </row>
     <row r="29" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C29" s="25" t="s">
+      <c r="C29" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="41"/>
       <c r="L29" s="15"/>
       <c r="M29" s="15"/>
       <c r="N29" s="15"/>
@@ -3844,103 +3844,123 @@
       <c r="R29" s="15"/>
     </row>
     <row r="30" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C30" s="25" t="s">
+      <c r="C30" s="41" t="s">
         <v>100</v>
       </c>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="25"/>
-      <c r="I30" s="25"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="41"/>
       <c r="L30" s="15"/>
     </row>
     <row r="31" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C31" s="25" t="s">
+      <c r="C31" s="41" t="s">
         <v>101</v>
       </c>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="41"/>
       <c r="L31" s="15"/>
     </row>
     <row r="32" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C32" s="25" t="s">
+      <c r="C32" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="25"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="41"/>
       <c r="L32" s="15"/>
     </row>
     <row r="33" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C33" s="25" t="s">
+      <c r="C33" s="41" t="s">
         <v>103</v>
       </c>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="25"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="41"/>
+      <c r="H33" s="41"/>
+      <c r="I33" s="41"/>
       <c r="L33" s="15"/>
     </row>
     <row r="34" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C34" s="25" t="s">
+      <c r="C34" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="25"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="41"/>
+      <c r="F34" s="41"/>
+      <c r="G34" s="41"/>
+      <c r="H34" s="41"/>
+      <c r="I34" s="41"/>
       <c r="L34" s="15"/>
     </row>
     <row r="35" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C35" s="25" t="s">
+      <c r="C35" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="25"/>
+      <c r="D35" s="41"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="41"/>
+      <c r="G35" s="41"/>
+      <c r="H35" s="41"/>
+      <c r="I35" s="41"/>
       <c r="L35" s="15"/>
     </row>
     <row r="36" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C36" s="25" t="s">
+      <c r="C36" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25"/>
-      <c r="H36" s="25"/>
-      <c r="I36" s="25"/>
+      <c r="D36" s="41"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
+      <c r="G36" s="41"/>
+      <c r="H36" s="41"/>
+      <c r="I36" s="41"/>
       <c r="L36" s="15"/>
     </row>
     <row r="37" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C37" s="25" t="s">
+      <c r="C37" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="25"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
+      <c r="G37" s="41"/>
+      <c r="H37" s="41"/>
+      <c r="I37" s="41"/>
       <c r="L37" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="C33:I33"/>
+    <mergeCell ref="C34:I34"/>
+    <mergeCell ref="C35:I35"/>
+    <mergeCell ref="C36:I36"/>
+    <mergeCell ref="C37:I37"/>
+    <mergeCell ref="C28:I28"/>
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="C30:I30"/>
+    <mergeCell ref="C31:I31"/>
+    <mergeCell ref="C32:I32"/>
+    <mergeCell ref="L14:P14"/>
+    <mergeCell ref="C24:I24"/>
+    <mergeCell ref="C25:I25"/>
+    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="C27:I27"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="L13:P13"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="P1:P2"/>
@@ -3954,26 +3974,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:H1"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="L13:P13"/>
-    <mergeCell ref="L14:P14"/>
-    <mergeCell ref="C24:I24"/>
-    <mergeCell ref="C25:I25"/>
-    <mergeCell ref="C26:I26"/>
-    <mergeCell ref="C27:I27"/>
-    <mergeCell ref="C28:I28"/>
-    <mergeCell ref="C29:I29"/>
-    <mergeCell ref="C30:I30"/>
-    <mergeCell ref="C31:I31"/>
-    <mergeCell ref="C32:I32"/>
-    <mergeCell ref="C33:I33"/>
-    <mergeCell ref="C34:I34"/>
-    <mergeCell ref="C35:I35"/>
-    <mergeCell ref="C36:I36"/>
-    <mergeCell ref="C37:I37"/>
   </mergeCells>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
completed first major version, waiting for feedback to start with the layout
</commit_message>
<xml_diff>
--- a/datasheets/uc/pinout.xlsx
+++ b/datasheets/uc/pinout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzahedi\Documents\Git\RoboFriend\datasheets\uc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8029D9ED-E9B8-4789-AB59-BE3F1940DE19}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E051D40E-B883-47EA-B761-590A3A99022C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="133">
   <si>
     <t>Ports</t>
   </si>
@@ -847,6 +847,9 @@
   </si>
   <si>
     <t>US3Trig</t>
+  </si>
+  <si>
+    <t>INA193</t>
   </si>
 </sst>
 </file>
@@ -1189,6 +1192,27 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1210,29 +1234,8 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1645,56 +1648,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="32" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
       <c r="J1"/>
       <c r="K1"/>
       <c r="L1"/>
-      <c r="M1" s="28" t="s">
+      <c r="M1" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="29" t="s">
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="31" t="s">
+      <c r="Q1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="31" t="s">
+      <c r="R1" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="S1" s="32" t="s">
+      <c r="S1" s="39" t="s">
         <v>108</v>
       </c>
       <c r="T1"/>
     </row>
     <row r="2" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
+      <c r="A2" s="42"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
       <c r="G2" s="2">
         <v>1</v>
       </c>
@@ -1716,17 +1719,17 @@
       <c r="O2" s="2">
         <v>1</v>
       </c>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="32"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="39"/>
       <c r="T2"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="41" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -1735,11 +1738,11 @@
       <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
       <c r="J3" s="3" t="s">
         <v>5</v>
       </c>
@@ -1747,11 +1750,11 @@
       <c r="L3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="35"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
       <c r="R3" s="18" t="s">
         <v>6</v>
       </c>
@@ -1761,8 +1764,8 @@
       <c r="T3"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
-      <c r="B4" s="34"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="24" t="s">
         <v>7</v>
       </c>
@@ -1809,10 +1812,10 @@
       <c r="T4"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="32" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -1863,8 +1866,8 @@
       <c r="T5"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="37"/>
-      <c r="B6" s="38"/>
+      <c r="A6" s="31"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="6" t="s">
         <v>21</v>
       </c>
@@ -1913,10 +1916,10 @@
       <c r="T6"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="34" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="19" t="s">
@@ -1965,8 +1968,8 @@
       <c r="T7"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="39"/>
-      <c r="B8" s="40"/>
+      <c r="A8" s="33"/>
+      <c r="B8" s="34"/>
       <c r="C8" s="19" t="s">
         <v>36</v>
       </c>
@@ -2203,11 +2206,11 @@
       <c r="L13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="M13" s="35"/>
-      <c r="N13" s="35"/>
-      <c r="O13" s="35"/>
-      <c r="P13" s="35"/>
-      <c r="Q13" s="35"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="29"/>
+      <c r="Q13" s="29"/>
       <c r="R13" s="18" t="s">
         <v>5</v>
       </c>
@@ -2239,11 +2242,11 @@
       <c r="L14" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="M14" s="35"/>
-      <c r="N14" s="35"/>
-      <c r="O14" s="35"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="35"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="29"/>
+      <c r="Q14" s="29"/>
       <c r="R14" s="18" t="s">
         <v>63</v>
       </c>
@@ -2530,7 +2533,7 @@
         <v>86</v>
       </c>
       <c r="K21"/>
-      <c r="L21" s="13" t="s">
+      <c r="L21" s="20" t="s">
         <v>88</v>
       </c>
       <c r="M21" s="4"/>
@@ -2544,8 +2547,10 @@
       <c r="Q21" s="4">
         <v>44</v>
       </c>
-      <c r="R21" s="4"/>
-      <c r="S21" s="13" t="s">
+      <c r="R21" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="S21" s="20" t="s">
         <v>88</v>
       </c>
       <c r="T21"/>
@@ -2610,16 +2615,16 @@
       <c r="T23"/>
     </row>
     <row r="24" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C24" s="41" t="s">
+      <c r="C24" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="41"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="41"/>
-      <c r="J24" s="41"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="28"/>
       <c r="M24" s="15"/>
       <c r="N24" s="16"/>
       <c r="O24" s="16"/>
@@ -2630,16 +2635,16 @@
       <c r="T24"/>
     </row>
     <row r="25" spans="3:20" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="42" t="s">
+      <c r="C25" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="42"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="30"/>
       <c r="M25" s="15"/>
       <c r="N25"/>
       <c r="O25"/>
@@ -2650,16 +2655,16 @@
       <c r="T25"/>
     </row>
     <row r="26" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C26" s="41" t="s">
+      <c r="C26" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
-      <c r="G26" s="41"/>
-      <c r="H26" s="41"/>
-      <c r="I26" s="41"/>
-      <c r="J26" s="41"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="28"/>
       <c r="M26" s="17"/>
       <c r="N26"/>
       <c r="O26"/>
@@ -2670,16 +2675,16 @@
       <c r="T26"/>
     </row>
     <row r="27" spans="3:20" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="42" t="s">
+      <c r="C27" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
       <c r="M27" s="15"/>
       <c r="N27" s="16"/>
       <c r="O27" s="16"/>
@@ -2690,16 +2695,16 @@
       <c r="T27" s="15"/>
     </row>
     <row r="28" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C28" s="41" t="s">
+      <c r="C28" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="41"/>
-      <c r="J28" s="41"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
       <c r="M28" s="15"/>
       <c r="N28" s="15"/>
       <c r="O28" s="15"/>
@@ -2710,16 +2715,16 @@
       <c r="T28" s="15"/>
     </row>
     <row r="29" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C29" s="41" t="s">
+      <c r="C29" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="D29" s="41"/>
-      <c r="E29" s="41"/>
-      <c r="F29" s="41"/>
-      <c r="G29" s="41"/>
-      <c r="H29" s="41"/>
-      <c r="I29" s="41"/>
-      <c r="J29" s="41"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="28"/>
       <c r="M29" s="15"/>
       <c r="N29" s="15"/>
       <c r="O29" s="15"/>
@@ -2730,131 +2735,111 @@
       <c r="T29" s="15"/>
     </row>
     <row r="30" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C30" s="41" t="s">
+      <c r="C30" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="41"/>
-      <c r="J30" s="41"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="28"/>
       <c r="M30" s="15"/>
     </row>
     <row r="31" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C31" s="41" t="s">
+      <c r="C31" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="D31" s="41"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="41"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="41"/>
-      <c r="I31" s="41"/>
-      <c r="J31" s="41"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="28"/>
       <c r="M31" s="15"/>
     </row>
     <row r="32" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C32" s="41" t="s">
+      <c r="C32" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="41"/>
-      <c r="I32" s="41"/>
-      <c r="J32" s="41"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="28"/>
       <c r="M32" s="15"/>
     </row>
     <row r="33" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C33" s="41" t="s">
+      <c r="C33" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="41"/>
-      <c r="I33" s="41"/>
-      <c r="J33" s="41"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="28"/>
+      <c r="J33" s="28"/>
       <c r="M33" s="15"/>
     </row>
     <row r="34" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C34" s="41" t="s">
+      <c r="C34" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="D34" s="41"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="41"/>
-      <c r="G34" s="41"/>
-      <c r="H34" s="41"/>
-      <c r="I34" s="41"/>
-      <c r="J34" s="41"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="28"/>
+      <c r="J34" s="28"/>
       <c r="M34" s="15"/>
     </row>
     <row r="35" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C35" s="41" t="s">
+      <c r="C35" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="D35" s="41"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
-      <c r="G35" s="41"/>
-      <c r="H35" s="41"/>
-      <c r="I35" s="41"/>
-      <c r="J35" s="41"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="28"/>
+      <c r="I35" s="28"/>
+      <c r="J35" s="28"/>
       <c r="M35" s="15"/>
     </row>
     <row r="36" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C36" s="41" t="s">
+      <c r="C36" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="D36" s="41"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
-      <c r="G36" s="41"/>
-      <c r="H36" s="41"/>
-      <c r="I36" s="41"/>
-      <c r="J36" s="41"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="28"/>
+      <c r="I36" s="28"/>
+      <c r="J36" s="28"/>
       <c r="M36" s="15"/>
     </row>
     <row r="37" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C37" s="41" t="s">
+      <c r="C37" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="D37" s="41"/>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
-      <c r="G37" s="41"/>
-      <c r="H37" s="41"/>
-      <c r="I37" s="41"/>
-      <c r="J37" s="41"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="28"/>
+      <c r="I37" s="28"/>
+      <c r="J37" s="28"/>
       <c r="M37" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="C33:J33"/>
-    <mergeCell ref="C34:J34"/>
-    <mergeCell ref="C35:J35"/>
-    <mergeCell ref="C36:J36"/>
-    <mergeCell ref="C37:J37"/>
-    <mergeCell ref="C28:J28"/>
-    <mergeCell ref="C29:J29"/>
-    <mergeCell ref="C30:J30"/>
-    <mergeCell ref="C31:J31"/>
-    <mergeCell ref="C32:J32"/>
-    <mergeCell ref="M14:Q14"/>
-    <mergeCell ref="C24:J24"/>
-    <mergeCell ref="C25:J25"/>
-    <mergeCell ref="C26:J26"/>
-    <mergeCell ref="C27:J27"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="M13:Q13"/>
     <mergeCell ref="M1:O1"/>
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="Q1:Q2"/>
@@ -2870,6 +2855,26 @@
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="R1:R2"/>
     <mergeCell ref="D1:D2"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="M13:Q13"/>
+    <mergeCell ref="M14:Q14"/>
+    <mergeCell ref="C24:J24"/>
+    <mergeCell ref="C25:J25"/>
+    <mergeCell ref="C26:J26"/>
+    <mergeCell ref="C27:J27"/>
+    <mergeCell ref="C28:J28"/>
+    <mergeCell ref="C29:J29"/>
+    <mergeCell ref="C30:J30"/>
+    <mergeCell ref="C31:J31"/>
+    <mergeCell ref="C32:J32"/>
+    <mergeCell ref="C33:J33"/>
+    <mergeCell ref="C34:J34"/>
+    <mergeCell ref="C35:J35"/>
+    <mergeCell ref="C36:J36"/>
+    <mergeCell ref="C37:J37"/>
   </mergeCells>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2897,24 +2902,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="32" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
       <c r="I1"/>
       <c r="J1"/>
       <c r="K1"/>
@@ -2926,7 +2931,7 @@
       <c r="O1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="31" t="s">
+      <c r="P1" s="38" t="s">
         <v>1</v>
       </c>
       <c r="Q1" s="44" t="s">
@@ -2935,11 +2940,11 @@
       <c r="R1"/>
     </row>
     <row r="2" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
+      <c r="A2" s="42"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
       <c r="F2" s="2">
         <v>1</v>
       </c>
@@ -2967,20 +2972,20 @@
       <c r="R2"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="41" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
       <c r="I3" s="10" t="s">
         <v>5</v>
       </c>
@@ -2988,19 +2993,19 @@
       <c r="K3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
       <c r="Q3" s="10" t="s">
         <v>6</v>
       </c>
       <c r="R3"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
-      <c r="B4" s="34"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
@@ -3041,10 +3046,10 @@
       <c r="R4"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="32" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -3089,8 +3094,8 @@
       <c r="R5"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="37"/>
-      <c r="B6" s="38"/>
+      <c r="A6" s="31"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="7" t="s">
         <v>21</v>
       </c>
@@ -3133,10 +3138,10 @@
       <c r="R6"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="34" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -3179,8 +3184,8 @@
       <c r="R7"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="39"/>
-      <c r="B8" s="40"/>
+      <c r="A8" s="33"/>
+      <c r="B8" s="34"/>
       <c r="C8" s="7" t="s">
         <v>36</v>
       </c>
@@ -3384,11 +3389,11 @@
       <c r="K13" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="L13" s="35"/>
-      <c r="M13" s="35"/>
-      <c r="N13" s="35"/>
-      <c r="O13" s="35"/>
-      <c r="P13" s="35"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="29"/>
       <c r="Q13" s="10" t="s">
         <v>5</v>
       </c>
@@ -3414,11 +3419,11 @@
       <c r="K14" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="35"/>
-      <c r="O14" s="35"/>
-      <c r="P14" s="35"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="29"/>
       <c r="Q14" s="10" t="s">
         <v>63</v>
       </c>
@@ -3736,15 +3741,15 @@
       <c r="R23"/>
     </row>
     <row r="24" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C24" s="41" t="s">
+      <c r="C24" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="41"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="41"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28"/>
       <c r="L24" s="15"/>
       <c r="M24" s="16"/>
       <c r="N24" s="16"/>
@@ -3754,15 +3759,15 @@
       <c r="R24"/>
     </row>
     <row r="25" spans="3:18" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="42" t="s">
+      <c r="C25" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
       <c r="L25" s="15"/>
       <c r="M25"/>
       <c r="N25"/>
@@ -3772,15 +3777,15 @@
       <c r="R25"/>
     </row>
     <row r="26" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C26" s="41" t="s">
+      <c r="C26" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
-      <c r="G26" s="41"/>
-      <c r="H26" s="41"/>
-      <c r="I26" s="41"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
       <c r="L26" s="17"/>
       <c r="M26"/>
       <c r="N26"/>
@@ -3790,15 +3795,15 @@
       <c r="R26"/>
     </row>
     <row r="27" spans="3:18" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="42" t="s">
+      <c r="C27" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
       <c r="L27" s="15"/>
       <c r="M27" s="16"/>
       <c r="N27" s="16"/>
@@ -3808,15 +3813,15 @@
       <c r="R27" s="15"/>
     </row>
     <row r="28" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C28" s="41" t="s">
+      <c r="C28" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="41"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
       <c r="L28" s="15"/>
       <c r="M28" s="15"/>
       <c r="N28" s="15"/>
@@ -3826,15 +3831,15 @@
       <c r="R28" s="15"/>
     </row>
     <row r="29" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C29" s="41" t="s">
+      <c r="C29" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="D29" s="41"/>
-      <c r="E29" s="41"/>
-      <c r="F29" s="41"/>
-      <c r="G29" s="41"/>
-      <c r="H29" s="41"/>
-      <c r="I29" s="41"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="28"/>
       <c r="L29" s="15"/>
       <c r="M29" s="15"/>
       <c r="N29" s="15"/>
@@ -3844,123 +3849,103 @@
       <c r="R29" s="15"/>
     </row>
     <row r="30" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C30" s="41" t="s">
+      <c r="C30" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="41"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
       <c r="L30" s="15"/>
     </row>
     <row r="31" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C31" s="41" t="s">
+      <c r="C31" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="D31" s="41"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="41"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="41"/>
-      <c r="I31" s="41"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="28"/>
       <c r="L31" s="15"/>
     </row>
     <row r="32" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C32" s="41" t="s">
+      <c r="C32" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="41"/>
-      <c r="I32" s="41"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="28"/>
       <c r="L32" s="15"/>
     </row>
     <row r="33" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C33" s="41" t="s">
+      <c r="C33" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="41"/>
-      <c r="I33" s="41"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="28"/>
       <c r="L33" s="15"/>
     </row>
     <row r="34" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C34" s="41" t="s">
+      <c r="C34" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="D34" s="41"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="41"/>
-      <c r="G34" s="41"/>
-      <c r="H34" s="41"/>
-      <c r="I34" s="41"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="28"/>
       <c r="L34" s="15"/>
     </row>
     <row r="35" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C35" s="41" t="s">
+      <c r="C35" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="D35" s="41"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
-      <c r="G35" s="41"/>
-      <c r="H35" s="41"/>
-      <c r="I35" s="41"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="28"/>
+      <c r="I35" s="28"/>
       <c r="L35" s="15"/>
     </row>
     <row r="36" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C36" s="41" t="s">
+      <c r="C36" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="D36" s="41"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
-      <c r="G36" s="41"/>
-      <c r="H36" s="41"/>
-      <c r="I36" s="41"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="28"/>
+      <c r="I36" s="28"/>
       <c r="L36" s="15"/>
     </row>
     <row r="37" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C37" s="41" t="s">
+      <c r="C37" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="D37" s="41"/>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
-      <c r="G37" s="41"/>
-      <c r="H37" s="41"/>
-      <c r="I37" s="41"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="28"/>
+      <c r="I37" s="28"/>
       <c r="L37" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="C33:I33"/>
-    <mergeCell ref="C34:I34"/>
-    <mergeCell ref="C35:I35"/>
-    <mergeCell ref="C36:I36"/>
-    <mergeCell ref="C37:I37"/>
-    <mergeCell ref="C28:I28"/>
-    <mergeCell ref="C29:I29"/>
-    <mergeCell ref="C30:I30"/>
-    <mergeCell ref="C31:I31"/>
-    <mergeCell ref="C32:I32"/>
-    <mergeCell ref="L14:P14"/>
-    <mergeCell ref="C24:I24"/>
-    <mergeCell ref="C25:I25"/>
-    <mergeCell ref="C26:I26"/>
-    <mergeCell ref="C27:I27"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="L13:P13"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="P1:P2"/>
@@ -3974,6 +3959,26 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:H1"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="L13:P13"/>
+    <mergeCell ref="L14:P14"/>
+    <mergeCell ref="C24:I24"/>
+    <mergeCell ref="C25:I25"/>
+    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="C27:I27"/>
+    <mergeCell ref="C28:I28"/>
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="C30:I30"/>
+    <mergeCell ref="C31:I31"/>
+    <mergeCell ref="C32:I32"/>
+    <mergeCell ref="C33:I33"/>
+    <mergeCell ref="C34:I34"/>
+    <mergeCell ref="C35:I35"/>
+    <mergeCell ref="C36:I36"/>
+    <mergeCell ref="C37:I37"/>
   </mergeCells>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>